<commit_message>
Adding global var + get fonctionnement
</commit_message>
<xml_diff>
--- a/src/main/resources/public/template/excel/template.xlsx
+++ b/src/main/resources/public/template/excel/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="18915" windowHeight="7230"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="18915" windowHeight="7230" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Investissement-LYCEES" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
-  <si>
-    <t>TOTAL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>LYCEES</t>
   </si>
@@ -39,19 +36,10 @@
     <t>CMR</t>
   </si>
   <si>
-    <t>Développement des TICE et des ENT</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
     <t xml:space="preserve">Récapitulatif fonctionnement </t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>N° CP 2019-455</t>
   </si>
   <si>
     <t>Demande Commentaire</t>
@@ -400,10 +388,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -412,12 +399,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -497,15 +478,23 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -522,16 +511,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -840,10 +823,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A2:G21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -851,29 +834,28 @@
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>9</v>
-      </c>
+    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="A3" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
+      <c r="A5" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -882,11 +864,11 @@
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
-        <v>1</v>
+      <c r="A8" s="33" t="s">
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -895,7 +877,7 @@
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
+      <c r="A9" s="33"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
@@ -1026,10 +1008,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A2:E10"/>
+  <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1037,41 +1019,38 @@
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
-    </row>
-    <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
+    </row>
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A4:E4"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1082,10 +1061,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:E47"/>
+  <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1093,44 +1072,38 @@
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
-    </row>
-    <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="36"/>
-    </row>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="38"/>
+    </row>
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A4:E4"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1141,61 +1114,50 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A2:B12"/>
+  <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="38"/>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
-    </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="45"/>
+    </row>
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1207,7 +1169,7 @@
   <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1219,218 +1181,216 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+    </row>
+    <row r="6" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="30">
+        <v>2351171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3">
+        <v>18</v>
+      </c>
+      <c r="D13" s="8">
+        <v>14004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8">
+        <v>14898</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-    </row>
-    <row r="6" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="D15" s="25">
+        <v>47402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="17"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+    </row>
+    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B20" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="33">
-        <v>2351171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="C20" s="20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="21">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-    </row>
-    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2</v>
-      </c>
-      <c r="D11" s="11">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="4">
-        <v>10</v>
-      </c>
-      <c r="D12" s="11">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="4">
-        <v>18</v>
-      </c>
-      <c r="D13" s="11">
-        <v>14004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="C21" s="20">
         <v>1</v>
       </c>
-      <c r="D14" s="11">
-        <v>14898</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="28">
-        <v>47402</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
+      <c r="D21" s="21">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-    </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="B22" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="23">
+      <c r="C22" s="20">
         <v>1</v>
       </c>
-      <c r="D20" s="24">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="23">
-        <v>1</v>
-      </c>
-      <c r="D21" s="24">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="23">
-        <v>1</v>
-      </c>
-      <c r="D22" s="24">
+      <c r="D22" s="21">
         <v>5200</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="28">
+      <c r="A23" s="17"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="25">
         <v>29200</v>
       </c>
     </row>
@@ -1452,7 +1412,7 @@
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1467,78 +1427,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="B7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
refactoring minors warnings and adding future classes
</commit_message>
<xml_diff>
--- a/src/main/resources/public/template/excel/template.xlsx
+++ b/src/main/resources/public/template/excel/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="18915" windowHeight="7230" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="18915" windowHeight="7230" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Investissement-LYCEES" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>LYCEES</t>
   </si>
@@ -42,21 +42,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Demande Commentaire</t>
-  </si>
-  <si>
-    <t>Quantité Accordée</t>
-  </si>
-  <si>
-    <t>Somme :</t>
-  </si>
-  <si>
-    <t>Libellé Demande</t>
-  </si>
-  <si>
-    <t>Somme Montant Accordé</t>
-  </si>
-  <si>
     <t>Récapitulatif des mesures engagées par imputation budgétaire</t>
   </si>
   <si>
@@ -82,63 +67,6 @@
   </si>
   <si>
     <t>Montant</t>
-  </si>
-  <si>
-    <t>94 - VITRY-SUR-SEINE JEAN-MACÉ (0940129E)</t>
-  </si>
-  <si>
-    <t>ASPIRATEUR MOBILE AVEC FILTRE DES FUMEES DE SOUDURE</t>
-  </si>
-  <si>
-    <t>aspirateur de fumées de soudure d'appoint pour le montage des pièces en dehors des zones couverte par la VMC.</t>
-  </si>
-  <si>
-    <t>MASQUE DE SOUDURE A CRISTAUX LIQUIDES</t>
-  </si>
-  <si>
-    <t>masques de soudure automatique pour la protection oculaire</t>
-  </si>
-  <si>
-    <t>MATERIEL DE MESURE</t>
-  </si>
-  <si>
-    <t>MICROSCOPE BINOCULAIRE</t>
-  </si>
-  <si>
-    <t>TABLE DE SOUDURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tables d'assemblage supplémentaires </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montant: </t>
-  </si>
-  <si>
-    <t>Programme : HP222-008 Équipement des lycées publics</t>
-  </si>
-  <si>
-    <t>Nature comptable : 236 - Participations financières aux lycées</t>
-  </si>
-  <si>
-    <t>Action  : 12200803 - Développement des TICE et des ENT</t>
-  </si>
-  <si>
-    <t>95 - MONTMORENCY JEAN-JACQUES ROUSSEAU (0950648N)</t>
-  </si>
-  <si>
-    <t>MATERIEL AUDIOVISUEL</t>
-  </si>
-  <si>
-    <t>équipements vidéo</t>
-  </si>
-  <si>
-    <t>Equipements audio</t>
-  </si>
-  <si>
-    <t>SYSTEME AFFICHAGE DYNAMIQUE</t>
-  </si>
-  <si>
-    <t>REMPLACER l'ancien panneau d'affichage ARACTICE HS et qui n'a jamais fonctionné convenablement</t>
   </si>
   <si>
     <t xml:space="preserve">Montant total des dotations financières </t>
@@ -151,10 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
-  </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -169,39 +94,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -247,18 +141,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -285,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -318,45 +206,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -385,137 +234,56 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -836,18 +604,18 @@
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -855,7 +623,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="3"/>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
@@ -864,7 +632,7 @@
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
@@ -877,7 +645,7 @@
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
+      <c r="A9" s="8"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
@@ -1020,18 +788,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1039,12 +807,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -1073,18 +841,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1092,12 +860,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
-        <v>40</v>
+      <c r="A8" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -1116,7 +884,7 @@
   </sheetPr>
   <dimension ref="A2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -1126,18 +894,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1145,10 +913,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
+      <c r="A8" s="14"/>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
+      <c r="A9" s="15"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -1166,10 +934,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A2:F23"/>
+  <dimension ref="A2:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1181,7 +949,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
@@ -1189,216 +957,19 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-    </row>
-    <row r="6" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="30">
-        <v>2351171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2</v>
-      </c>
-      <c r="D11" s="8">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="3">
-        <v>10</v>
-      </c>
-      <c r="D12" s="8">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3">
-        <v>18</v>
-      </c>
-      <c r="D13" s="8">
-        <v>14004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8">
-        <v>14898</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="25">
-        <v>47402</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-    </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="20">
-        <v>1</v>
-      </c>
-      <c r="D20" s="21">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="20">
-        <v>1</v>
-      </c>
-      <c r="D21" s="21">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="20">
-        <v>1</v>
-      </c>
-      <c r="D22" s="21">
-        <v>5200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="25">
-        <v>29200</v>
-      </c>
-    </row>
+      <c r="A4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="6" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1427,76 +998,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="G7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="H7" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>